<commit_message>
doe review in progress
</commit_message>
<xml_diff>
--- a/Ariba Error Report_Performer/Data/Config.xlsx
+++ b/Ariba Error Report_Performer/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubAnkush\Ariba-Error-Report\Ariba Error Report_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AB9D49-9031-4032-B78D-D696AEA530A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -160,6 +157,87 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>SQ01_ClearDocsUsergroup</t>
+  </si>
+  <si>
+    <t>SQ01_ClearDocsQuery</t>
+  </si>
+  <si>
+    <t>SQ01_AribaInvoiceUsergroup</t>
+  </si>
+  <si>
+    <t>SQ01_AribaInvoiceQuery</t>
+  </si>
+  <si>
+    <t>ZCREDIT</t>
+  </si>
+  <si>
+    <t>CLEAREDDOCS</t>
+  </si>
+  <si>
+    <t>ZTWCMASTER</t>
+  </si>
+  <si>
+    <t>ARIBAINVINFO</t>
+  </si>
+  <si>
+    <t>SQ01_ClearDocsCompanyCode</t>
+  </si>
+  <si>
+    <t>TWC1</t>
+  </si>
+  <si>
+    <t>SQ01_AribaInvoicePrecedingValue1</t>
+  </si>
+  <si>
+    <t>SQ01_AribaInvoicePrecedingValue2</t>
+  </si>
+  <si>
+    <t>1*</t>
+  </si>
+  <si>
+    <t>8*</t>
+  </si>
+  <si>
+    <t>Ariba Error Report-Performer</t>
+  </si>
+  <si>
+    <t>SAPFile_Location</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\SAP\FrontEnd\SAPgui\saplogon.exe</t>
+  </si>
+  <si>
+    <t>SAP_server</t>
+  </si>
+  <si>
+    <t>ERP</t>
+  </si>
+  <si>
+    <t>SAP_Credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP_Client </t>
+  </si>
+  <si>
+    <t>TenantID</t>
+  </si>
+  <si>
+    <t>SecretID</t>
+  </si>
+  <si>
+    <t>ApplicationID</t>
+  </si>
+  <si>
+    <t>SuccessEmail</t>
+  </si>
+  <si>
+    <t>ExceptionEmail</t>
+  </si>
+  <si>
+    <t>CcEmail</t>
   </si>
 </sst>
 </file>
@@ -211,15 +289,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -239,9 +320,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +360,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +466,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +608,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -538,15 +619,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -585,34 +666,34 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1617,18 +1698,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1746,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1673,18 +1754,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1789,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1811,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1822,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,86 +1833,177 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="5">
+        <v>400</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -2765,13 +2937,6 @@
     <row r="979" ht="14.25" customHeight="1"/>
     <row r="980" ht="14.25" customHeight="1"/>
     <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2782,14 +2947,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2800,7 +2967,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2828,10 +2995,29 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
main testing in progress
</commit_message>
<xml_diff>
--- a/Ariba Error Report_Performer/Data/Config.xlsx
+++ b/Ariba Error Report_Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubAnkush\Ariba-Error-Report\Ariba Error Report_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AB9D49-9031-4032-B78D-D696AEA530A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CABB5C-E1EE-46E4-B533-6EC4EBADD800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,25 @@
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -219,9 +232,6 @@
     <t>SAP_Credentials</t>
   </si>
   <si>
-    <t xml:space="preserve">SAP_Client </t>
-  </si>
-  <si>
     <t>TenantID</t>
   </si>
   <si>
@@ -238,6 +248,42 @@
   </si>
   <si>
     <t>CcEmail</t>
+  </si>
+  <si>
+    <t>SAP_Client</t>
+  </si>
+  <si>
+    <t>SuccessEmail_Ariba</t>
+  </si>
+  <si>
+    <t>ExceptionEmail_Ariba</t>
+  </si>
+  <si>
+    <t>CcEmail_Ariba</t>
+  </si>
+  <si>
+    <t>EmailSubject_SException</t>
+  </si>
+  <si>
+    <t>EmailSubject_BException</t>
+  </si>
+  <si>
+    <t>EmailSubject_Success</t>
+  </si>
+  <si>
+    <t>System Exception - Ariba Error Report performer</t>
+  </si>
+  <si>
+    <t>Business Exception - Ariba Error Report performer</t>
+  </si>
+  <si>
+    <t>Ariba Invoices Need Attention</t>
+  </si>
+  <si>
+    <t>EmailBody_Success</t>
+  </si>
+  <si>
+    <t>Attached is the list of Ariba invoices that are not paid, approved or sent for the previous week.</t>
   </si>
 </sst>
 </file>
@@ -1700,14 +1746,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:B32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -1909,7 +1955,7 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B22" s="5">
         <v>400</v>
@@ -1977,26 +2023,54 @@
     <row r="33" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2997,25 +3071,34 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Code rview in progress
</commit_message>
<xml_diff>
--- a/Ariba Error Report_Performer/Data/Config.xlsx
+++ b/Ariba Error Report_Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubAnkush\Ariba-Error-Report\Ariba Error Report_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CABB5C-E1EE-46E4-B533-6EC4EBADD800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7631621-E6FD-4BC9-AA04-A143B510A05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -284,6 +284,15 @@
   </si>
   <si>
     <t>Attached is the list of Ariba invoices that are not paid, approved or sent for the previous week.</t>
+  </si>
+  <si>
+    <t>WE05AribaInvoiceFileSheetName</t>
+  </si>
+  <si>
+    <t>ZcreditClearedAribaFileSheetName</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
   </si>
 </sst>
 </file>
@@ -1746,8 +1755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2073,8 +2082,22 @@
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
submitted main for code review
</commit_message>
<xml_diff>
--- a/Ariba Error Report_Performer/Data/Config.xlsx
+++ b/Ariba Error Report_Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubAnkush\Ariba-Error-Report\Ariba Error Report_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7631621-E6FD-4BC9-AA04-A143B510A05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242090AB-D820-4797-8DB2-3C90AF64B3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -169,9 +169,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
     <t>SQ01_ClearDocsUsergroup</t>
   </si>
   <si>
@@ -293,6 +290,15 @@
   </si>
   <si>
     <t>Sheet1</t>
+  </si>
+  <si>
+    <t>InvoiceInfoSheetName</t>
+  </si>
+  <si>
+    <t>Sheet2</t>
+  </si>
+  <si>
+    <t>Ariba Error Report</t>
   </si>
 </sst>
 </file>
@@ -673,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -724,7 +730,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -745,7 +751,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -1755,8 +1761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1940,31 +1946,31 @@
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
         <v>59</v>
-      </c>
-      <c r="B19" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
         <v>61</v>
-      </c>
-      <c r="B20" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" s="5">
         <v>400</v>
@@ -1973,132 +1979,139 @@
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
         <v>52</v>
-      </c>
-      <c r="B26" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1">
       <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" t="s">
         <v>80</v>
-      </c>
-      <c r="B41" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="44" spans="1:2" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1">
       <c r="A45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" t="s">
         <v>83</v>
       </c>
-      <c r="B45" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A46" t="s">
         <v>84</v>
       </c>
+      <c r="B46" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
@@ -3094,34 +3107,34 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>